<commit_message>
new exponentiel to calculate the power for each glass sections
</commit_message>
<xml_diff>
--- a/LaboInsru/position/dataA.xlsx
+++ b/LaboInsru/position/dataA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Documents\GitHub\Academic\LaboInsru\position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41175268-2C96-44F6-B1BE-712D36CAFDDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC65061C-1A67-45D3-A363-70220E365A1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="257" yWindow="463" windowWidth="30394" windowHeight="14708" xr2:uid="{B295DECF-01BD-4365-A2B3-C3AC1600456C}"/>
+    <workbookView xWindow="360" yWindow="972" windowWidth="30396" windowHeight="14712" activeTab="1" xr2:uid="{B295DECF-01BD-4365-A2B3-C3AC1600456C}"/>
   </bookViews>
   <sheets>
     <sheet name="position" sheetId="1" r:id="rId1"/>
@@ -6994,7 +6994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57C5F7A-085D-463D-A7EC-C7D39B7CE96D}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
@@ -8015,8 +8015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6077946E-23BD-4FEC-A4D5-4F2A491EA003}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>